<commit_message>
Update Paralelo 3 Notas y Asistencias (1).xlsx
</commit_message>
<xml_diff>
--- a/AYUDANTIA/Paralelo 3 Notas y Asistencias (1).xlsx
+++ b/AYUDANTIA/Paralelo 3 Notas y Asistencias (1).xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\4to Sync\4to-Semestre\AYUDANTIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AD5B3F90-BA4D-4BCD-B488-98F300450300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF4D2B5-B618-4ACA-8150-7D0A9AAC8567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notas_Deberes" sheetId="1" r:id="rId1"/>
     <sheet name="Notas_Colaborativos" sheetId="3" r:id="rId2"/>
     <sheet name="Asistencias_Tutorias" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="64">
   <si>
     <t>Nombre</t>
   </si>
@@ -211,12 +211,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>DeberOpcional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14">
     <font>
       <sz val="10"/>
@@ -407,27 +410,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="Accent" xfId="2"/>
-    <cellStyle name="Accent 1" xfId="3"/>
-    <cellStyle name="Accent 2" xfId="4"/>
-    <cellStyle name="Accent 3" xfId="5"/>
-    <cellStyle name="Bad" xfId="6"/>
-    <cellStyle name="Default" xfId="7"/>
-    <cellStyle name="Error" xfId="8"/>
-    <cellStyle name="Footnote" xfId="9"/>
-    <cellStyle name="Good" xfId="10"/>
-    <cellStyle name="Heading" xfId="11"/>
-    <cellStyle name="Heading 1" xfId="12"/>
-    <cellStyle name="Heading 2" xfId="13"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
+    <cellStyle name="Accent" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Default" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Error" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Footnote" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Good" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Heading" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Heading 1" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Heading 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="15"/>
-    <cellStyle name="Result" xfId="16"/>
-    <cellStyle name="Result2" xfId="17"/>
-    <cellStyle name="Status" xfId="18"/>
-    <cellStyle name="Text" xfId="19"/>
-    <cellStyle name="Warning" xfId="20"/>
+    <cellStyle name="Note" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Result" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Result2" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Status" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Text" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Warning" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -758,11 +761,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="12.75"/>
@@ -1346,26 +1349,240 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
@@ -1375,7 +1592,7 @@
     <col min="16378" max="16384" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1606,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1400,7 +1617,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1414,7 +1631,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.75">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1422,7 +1639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1430,7 +1647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1438,7 +1655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1449,7 +1666,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.75">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1457,7 +1674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.75">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1468,7 +1685,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.75">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +1693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.75">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1484,7 +1701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12.75">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1492,7 +1709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="12.75">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.75">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1511,7 +1728,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1519,7 +1736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="12.75">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1527,7 +1744,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12.75">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1538,7 +1755,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12.75">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1549,7 +1766,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12.75">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1560,7 +1777,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="12.75">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1568,7 +1785,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12.75">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1576,7 +1793,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12.75">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1587,7 +1804,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12.75">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1598,7 +1815,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12.75">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1606,7 +1823,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="12.75">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1617,7 +1834,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12.75">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>50</v>
       </c>

</xml_diff>